<commit_message>
Revisions to the Part Required Field validation.
</commit_message>
<xml_diff>
--- a/Validation/Part/PartRequiredFieldValidation - Template.xlsx
+++ b/Validation/Part/PartRequiredFieldValidation - Template.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>PartID</t>
   </si>
@@ -67,6 +67,39 @@
   </si>
   <si>
     <t>PART_GROUP</t>
+  </si>
+  <si>
+    <t>NewDescription</t>
+  </si>
+  <si>
+    <t>Cat</t>
+  </si>
+  <si>
+    <t>PartsClassID</t>
+  </si>
+  <si>
+    <t>CurrentDescription</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>U/I</t>
+  </si>
+  <si>
+    <t>AW_StockStatus</t>
+  </si>
+  <si>
+    <t>NewMfgNo</t>
+  </si>
+  <si>
+    <t>Bin1</t>
+  </si>
+  <si>
+    <t>Bin2</t>
+  </si>
+  <si>
+    <t>Bin3</t>
   </si>
 </sst>
 </file>
@@ -395,7 +428,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:AB1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -403,12 +436,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" customWidth="1"/>
     <col min="6" max="6" width="17.7109375" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.28515625" customWidth="1"/>
     <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
@@ -416,9 +450,14 @@
     <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -466,6 +505,42 @@
       </c>
       <c r="P1" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>